<commit_message>
connect speech rec to distance
</commit_message>
<xml_diff>
--- a/схема.xlsx
+++ b/схема.xlsx
@@ -38,9 +38,6 @@
     <t>В поддержку новичкам реализована программа помогатор, в рамках которой студенты могут помогать отстающим</t>
   </si>
   <si>
-    <t>Стипендия есть у студентов, учащихся на бюджете, до первой сессии она есть у всех первокурсников и равна стипендии для студентов, сдавших сессию на 4 и 5. После первой сессии для студентов, сдавших сессию на 4 и 5 она составляет, по последним данным, 3383 рубля, для сдавших сессию на 5 - 5751 рубль. Сумма стипендии иногда меняется, поэтому советую отслеживать новости в группе профкома фсир в вк</t>
-  </si>
-  <si>
     <t>Для школьников проводятся дни открытых дверей, на которых можно узнать всю необходимую информацию о факультете, задать вопросы, больше узнать о программе прикладной информатики</t>
   </si>
   <si>
@@ -93,6 +90,9 @@
   </si>
   <si>
     <t>какие рядом магазины</t>
+  </si>
+  <si>
+    <t>Стипендия есть у студентов, учащихся на бюджете, до первой сессии она есть у всех первокурсников и равна стипендии для студентов, сдавших сессию на 4 и 5. После первой сессии для студентов, сдавших сессию на 4 и 5 она составляет, по последним данным, 3200 рублей, для сдавших сессию на 5 - 5600 рублей. Сумма стипендии иногда меняется, поэтому советую отслеживать новости в группе профкома фсир в вк</t>
   </si>
 </sst>
 </file>
@@ -439,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,7 +452,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -460,7 +460,7 @@
     </row>
     <row r="2" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>2</v>
@@ -476,7 +476,7 @@
     </row>
     <row r="4" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>3</v>
@@ -484,72 +484,72 @@
     </row>
     <row r="5" spans="1:2" ht="216" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="216" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="216" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="216" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="216" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add not finished emoji
</commit_message>
<xml_diff>
--- a/схема.xlsx
+++ b/схема.xlsx
@@ -47,9 +47,6 @@
     <t>где находится корпус</t>
   </si>
   <si>
-    <t>есть ли в корпусе столовая</t>
-  </si>
-  <si>
     <t>какие мероприятия есть на факультете</t>
   </si>
   <si>
@@ -83,9 +80,6 @@
     <t>корпус №6 лермонтова 126, главный корпус рядом с белый домом</t>
   </si>
   <si>
-    <t>Ахахах, о еде $$удивление + улыбка$$. В корпусе на первом этаже есть столовая и автомат с кофе $$улыбка$$, также прямо на остановке факультета есть киоск, выше по склону слата, и в библиотеке, где ты можешь ещё и почитать, есть столовая, где можно полноценно покушать.</t>
-  </si>
-  <si>
     <t>Иногда на факультете проводятся клубные тусовки, где ты можешь потанцевать и подвигаться. $$поднимает брови$$Но есть и милые ламповые встречи, например, мне по душе пришелся вечер стихов при тусклом свете и пением под гитару. $$мечтательная улыбка$$ К тому же, проводятся выступления по поводу окончания семестра, например, недавно была "мисс весна", где выступали вокалистки факультета $$поднимает брови$$</t>
   </si>
   <si>
@@ -135,6 +129,12 @@
   </si>
   <si>
     <t>удачи</t>
+  </si>
+  <si>
+    <t>где в корпусе столовая</t>
+  </si>
+  <si>
+    <t>Ахахах, о еде. $$удивление $$улыбка  В корпусе на первом этаже есть столовая и автомат с кофе, $$улыбка также прямо на остановке факультета есть киоск, выше по склону слата, и в библиотеке, где ты можешь ещё и почитать, есть столовая, где можно полноценно покушать.</t>
   </si>
 </sst>
 </file>
@@ -481,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -497,10 +497,10 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
@@ -508,21 +508,21 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
@@ -533,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="216" x14ac:dyDescent="0.3">
@@ -541,21 +541,21 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -563,81 +563,81 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="216" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="216" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
at least i tried
every logics works in logics(ex main), return 3 val: emoji, answer and sound_name
</commit_message>
<xml_diff>
--- a/схема.xlsx
+++ b/схема.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -65,27 +66,15 @@
     <t>Стипендия есть у студентов, учащихся на бюджете, до первой сессии она есть у всех первокурсников и равна стипендии для студентов, сдавших сессию на 4 и 5. После первой сессии для студентов, сдавших сессию на 4 и 5 она составляет, по последним данным, 3200 рублей, для сдавших сессию на 5 - 5600 рублей. Сумма стипендии иногда меняется, поэтому советую отслеживать новости в группе профкома фсир в вк</t>
   </si>
   <si>
-    <t>Предметы расставлены в приоритете: информатика, математика, русский язык</t>
-  </si>
-  <si>
     <t>На сайте иркутского государственного университета есть информация о самом университете, а также о факультете сервиса и рекламы</t>
   </si>
   <si>
-    <t>Есть возможность изучать польский, некоторые студенты после этого могут поехать по обмену в Польшу; французский или испанский, для направления туризм; английский в рамках учебной программы</t>
-  </si>
-  <si>
     <t>когда можно прийти посмотреть факультет</t>
   </si>
   <si>
-    <t>корпус №6 лермонтова 126, главный корпус рядом с белый домом</t>
-  </si>
-  <si>
     <t>Иногда на факультете проводятся клубные тусовки, где ты можешь потанцевать и подвигаться. $$поднимает брови$$Но есть и милые ламповые встречи, например, мне по душе пришелся вечер стихов при тусклом свете и пением под гитару. $$мечтательная улыбка$$ К тому же, проводятся выступления по поводу окончания семестра, например, недавно была "мисс весна", где выступали вокалистки факультета $$поднимает брови$$</t>
   </si>
   <si>
-    <t>Слата выше по склону и киоск прямо на остановке</t>
-  </si>
-  <si>
     <t>Для удобства студентов создан форлабс, электронная база, где можно отследить свои баллы по предметам, посмотреть или прикрепить домашнее задание, написать преподавателю или пройти тест или контрольную в режиме онлайн. Для прикладников, и конечно для всех желающих существует возможность создания своих проектов в лаборатории, общение со старшими курсами, которые могут помочь и рассказать что-то полезное</t>
   </si>
   <si>
@@ -135,6 +124,18 @@
   </si>
   <si>
     <t>Ахахах, о еде. $$удивление $$улыбка  В корпусе на первом этаже есть столовая и автомат с кофе, $$улыбка также прямо на остановке факультета есть киоск, выше по склону слата, и в библиотеке, где ты можешь ещё и почитать, есть столовая, где можно полноценно покушать.</t>
+  </si>
+  <si>
+    <t>Предметы расставлены в приоритете: информатика, математика, русский язык $хитрость</t>
+  </si>
+  <si>
+    <t>Есть возможность изучать польский, некоторые студенты после этого могут поехать по обмену в Польшу; французский или испанский, для направления туризм; английский в рамках учебной программы $$хитрость</t>
+  </si>
+  <si>
+    <t>корпус №6 лермонтова 126, главный корпус рядом с белый домом $$уточка</t>
+  </si>
+  <si>
+    <t>Слата выше по склону и киоск прямо на остановке $$хитрость</t>
   </si>
 </sst>
 </file>
@@ -481,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -492,15 +493,15 @@
     <col min="3" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
@@ -508,10 +509,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
@@ -519,10 +520,10 @@
         <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
@@ -533,7 +534,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="216" x14ac:dyDescent="0.3">
@@ -544,18 +545,18 @@
         <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -563,21 +564,21 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="201.6" x14ac:dyDescent="0.3">
@@ -585,10 +586,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="201.6" x14ac:dyDescent="0.3">
@@ -596,10 +597,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="201.6" x14ac:dyDescent="0.3">
@@ -607,10 +608,10 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -618,26 +619,26 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="216" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="216" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>